<commit_message>
auto insert pdf files from attachments folder
</commit_message>
<xml_diff>
--- a/data_for_sending.xlsx
+++ b/data_for_sending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\SKILLBOX\Mailer\mailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F2D199-A2A0-4D07-A698-18A9A454A4C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE52598-BF02-4206-8166-BCB63280AB18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
-  <si>
-    <t>This is test subject</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>email</t>
   </si>
@@ -42,37 +39,20 @@
     <t>attachment</t>
   </si>
   <si>
-    <t>testatt1.pdf</t>
-  </si>
-  <si>
-    <t>testatt2.pdf</t>
-  </si>
-  <si>
-    <t>testatt3.pdf</t>
-  </si>
-  <si>
-    <t>testatt4.pdf</t>
-  </si>
-  <si>
-    <t>Test text</t>
+    <t>Test subject</t>
+  </si>
+  <si>
+    <t>Test text body</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -86,15 +66,7 @@
       <charset val="204"/>
     </font>
     <font>
-      <u/>
-      <sz val="14"/>
-      <color theme="10"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="14"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Tahoma"/>
       <family val="2"/>
@@ -139,21 +111,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Гиперссылка" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -434,75 +408,67 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" customWidth="1"/>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
+    <col min="2" max="2" width="59.140625" customWidth="1"/>
+    <col min="3" max="3" width="128.140625" customWidth="1"/>
     <col min="4" max="4" width="77.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="234.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="3"/>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>5</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3" t="s">
-        <v>6</v>
-      </c>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="3"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="2"/>
       <c r="C5" s="4"/>
-      <c r="D5" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="D5" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix for copying to sent folder
</commit_message>
<xml_diff>
--- a/data_for_sending.xlsx
+++ b/data_for_sending.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\k14\Desktop\My Java Apps\Mailer\mailer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A1048C-3281-4AB8-BAFD-98272BDFCD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E7CADB-00A4-40C3-BC2A-8E262960E84B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>email</t>
   </si>
@@ -39,41 +39,20 @@
     <t>attachment</t>
   </si>
   <si>
-    <t>pmbakanov@mid.ru</t>
-  </si>
-  <si>
-    <t>pashtetrus@gmail.com</t>
-  </si>
-  <si>
-    <t>pashtet_rus@mail.ru</t>
-  </si>
-  <si>
     <t>Test subject</t>
   </si>
   <si>
     <t>Test text</t>
-  </si>
-  <si>
-    <t>Amazon.com - Order 114-7674838-7234659.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -93,6 +72,14 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -108,7 +95,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -131,59 +118,28 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -469,18 +425,18 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="43.59765625"/>
-    <col min="2" max="2" customWidth="true" width="59.1328125"/>
-    <col min="3" max="3" customWidth="true" width="128.1328125"/>
-    <col min="4" max="4" customWidth="true" width="77.265625"/>
+    <col min="1" max="1" width="26.73046875" customWidth="1"/>
+    <col min="2" max="2" width="59.1328125" customWidth="1"/>
+    <col min="3" max="3" width="128.1328125" customWidth="1"/>
+    <col min="4" max="4" width="77.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.45">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -494,47 +450,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="234.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:4" ht="234.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6"/>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="0">
-        <v>9</v>
+      <c r="C2" s="5" t="s">
+        <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="5" t="s">
-        <v>5</v>
-      </c>
+    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="6"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
-      <c r="D3" t="s" s="0">
-        <v>9</v>
-      </c>
     </row>
-    <row r="4" spans="1:4" ht="17.649999999999999" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="5" t="s">
-        <v>6</v>
-      </c>
+    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="3"/>
       <c r="B4" s="1"/>
       <c r="C4" s="2"/>
-      <c r="D4" t="s" s="0">
-        <v>9</v>
-      </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{3EC57BE1-2AD2-462B-9154-81B6DE35D650}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{FAC4998A-2F74-440B-9F7C-F00B95F89A63}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{5EA9CE38-5C69-4188-A5EE-3D5256069DF7}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>